<commit_message>
Filesize Correction Adc Keypad
</commit_message>
<xml_diff>
--- a/Proximab.xlsx
+++ b/Proximab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/31031dea7aa373a1/Belgeler/Arduino/Proximab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{50160C59-8F57-4107-827B-BBF55579F6E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23516467-C0EF-4099-B3E3-19D86B47987C}"/>
+  <xr:revisionPtr revIDLastSave="507" documentId="13_ncr:1_{50160C59-8F57-4107-827B-BBF55579F6E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9377A87-C5B6-414C-9E66-2D35B45BEC48}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Menu3" sheetId="4" r:id="rId3"/>
     <sheet name="MenuF" sheetId="5" r:id="rId4"/>
     <sheet name="UI" sheetId="3" r:id="rId5"/>
+    <sheet name="Key" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="211">
   <si>
     <t xml:space="preserve">Enter </t>
   </si>
@@ -608,12 +609,96 @@
   <si>
     <t>Ser: 115200 baud NL&amp;CR</t>
   </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Adc</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>Kohm</t>
+  </si>
+  <si>
+    <t>adc</t>
+  </si>
+  <si>
+    <t>S1 S2</t>
+  </si>
+  <si>
+    <t>S1 S3</t>
+  </si>
+  <si>
+    <t>S1 S4</t>
+  </si>
+  <si>
+    <t>S2 S3</t>
+  </si>
+  <si>
+    <t>S2 S4</t>
+  </si>
+  <si>
+    <t>S3 S4</t>
+  </si>
+  <si>
+    <t>S1 S2 S3</t>
+  </si>
+  <si>
+    <t>S1 S2 S4</t>
+  </si>
+  <si>
+    <t>S2 S3 S4</t>
+  </si>
+  <si>
+    <t>S1 S3 S4</t>
+  </si>
+  <si>
+    <t>Fix R1</t>
+  </si>
+  <si>
+    <t>Fix R6</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>mVolt</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,6 +717,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -801,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -847,6 +945,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -870,6 +975,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7FE3028-44F3-4774-9F33-4D89D4C0C53B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8477250" y="466725"/>
+          <a:ext cx="2286000" cy="5686425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1231,14 +1402,14 @@
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
         <v>3</v>
@@ -1252,15 +1423,15 @@
       <c r="S4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="31" t="s">
+      <c r="T4" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="37"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -2407,7 +2578,7 @@
   <dimension ref="A2:AC44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,14 +2646,14 @@
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
         <v>3</v>
@@ -2505,15 +2676,15 @@
       <c r="S4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="31" t="s">
+      <c r="T4" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="37"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -3596,8 +3767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E648633-5BB0-4FFA-AB25-4F6B5B222844}">
   <dimension ref="A2:AC44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:P8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3665,14 +3836,14 @@
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="29" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
         <v>3</v>
@@ -3695,15 +3866,15 @@
       <c r="S4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="31" t="s">
+      <c r="T4" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="31"/>
-      <c r="V4" s="31"/>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31"/>
-      <c r="Z4" s="32"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="37"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -4893,7 +5064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F7F362-1500-415B-8742-4DD6E6C5F9F7}">
   <dimension ref="B2:R35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -6335,4 +6506,525 @@
     <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Classified as Internal</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39401F82-8C98-40FD-BFA6-89650728085B}">
+  <dimension ref="K1:U34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB24" sqref="AB24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" style="31" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" style="29" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" style="5" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="33" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="3"/>
+    <col min="18" max="18" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O1" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="P1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="R1" s="5">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>193</v>
+      </c>
+      <c r="U1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O2" s="33">
+        <v>5000</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1024</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="R2" s="5">
+        <v>22</v>
+      </c>
+      <c r="S2" t="s">
+        <v>193</v>
+      </c>
+      <c r="U2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="R3" s="5">
+        <v>47</v>
+      </c>
+      <c r="S3" t="s">
+        <v>193</v>
+      </c>
+      <c r="U3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="R4" s="5">
+        <v>10</v>
+      </c>
+      <c r="S4" t="s">
+        <v>193</v>
+      </c>
+      <c r="U4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="R5" s="5">
+        <v>47</v>
+      </c>
+      <c r="S5" t="s">
+        <v>193</v>
+      </c>
+      <c r="U5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>193</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="T9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="S10">
+        <v>22</v>
+      </c>
+      <c r="T10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="S11">
+        <v>22</v>
+      </c>
+      <c r="T11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <v>39</v>
+      </c>
+      <c r="T12">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="O13" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="P13" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="S13">
+        <v>10</v>
+      </c>
+      <c r="T13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>204</v>
+      </c>
+      <c r="M14" s="29">
+        <f>P2*(0+R6)/(R1+R2+R3+R4+R5+R6)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O14" s="33">
+        <f>(O2/P2)*M14</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="29">
+        <f t="shared" ref="P14:P16" si="0">M14-M13</f>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>47</v>
+      </c>
+      <c r="T14">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15" s="29">
+        <f>P2*(0+R6)/(R1+R2+R3+R4+R5+R6)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O15" s="33">
+        <f>(O2/P2)*M15</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="12:21" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>200</v>
+      </c>
+      <c r="M16" s="29">
+        <f>P2*(0+R6)/(R1+R2+R3+R4+R5+R6)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O16" s="33">
+        <f>(O2/P2)*M16</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L17" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="M17" s="30">
+        <f>P2*(R4+R6)/(R1+R2+R3+R4+R6)</f>
+        <v>101.38613861386139</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O17" s="30">
+        <f>(O2/P2)*M17</f>
+        <v>495.04950495049508</v>
+      </c>
+      <c r="P17" s="30">
+        <f>M17-M16</f>
+        <v>101.38613861386139</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>197</v>
+      </c>
+      <c r="M18" s="29">
+        <f>P2*(R4+R6)/(R1+R3+R4+R6)</f>
+        <v>129.62025316455697</v>
+      </c>
+      <c r="N18" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O18" s="33">
+        <f>(O2/P2)*M18</f>
+        <v>632.91139240506334</v>
+      </c>
+      <c r="P18" s="30">
+        <f t="shared" ref="P18:P28" si="1">M18-M17</f>
+        <v>28.23411455069558</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>199</v>
+      </c>
+      <c r="M19" s="29">
+        <f>P2*(R4+R6)/(R1+R2+R4+R6)</f>
+        <v>189.62962962962962</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O19" s="33">
+        <f>(O2/P2)*M19</f>
+        <v>925.92592592592587</v>
+      </c>
+      <c r="P19" s="29">
+        <f t="shared" si="1"/>
+        <v>60.009376465072648</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L20" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="M20" s="30">
+        <f>P2*(R5+R6)/(R1+R2+R3+R5+R6)</f>
+        <v>348.75362318840581</v>
+      </c>
+      <c r="N20" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O20" s="30">
+        <f>(O2/P2)*M20</f>
+        <v>1702.8985507246377</v>
+      </c>
+      <c r="P20" s="30">
+        <f t="shared" si="1"/>
+        <v>159.12399355877619</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L21" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="M21" s="30">
+        <f>P2*(R4+R5+R6)/(R1+R2+R3+R4+R5+R6)</f>
+        <v>394.37837837837839</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O21" s="30">
+        <f>(O2/P2)*M21</f>
+        <v>1925.6756756756756</v>
+      </c>
+      <c r="P21" s="30">
+        <f t="shared" si="1"/>
+        <v>45.624755189972575</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="22" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>202</v>
+      </c>
+      <c r="M22" s="29">
+        <f>P2*(R4+R6)/(R1+R4+R6)</f>
+        <v>320</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O22" s="33">
+        <f>(O2/P2)*M22</f>
+        <v>1562.5</v>
+      </c>
+      <c r="P22" s="30">
+        <f t="shared" si="1"/>
+        <v>-74.378378378378386</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>196</v>
+      </c>
+      <c r="M23" s="29">
+        <f>P2*(R5+R6)/(R1+R3+R5+R6)</f>
+        <v>414.89655172413791</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O23" s="33">
+        <f>(O2/P2)*M23</f>
+        <v>2025.8620689655172</v>
+      </c>
+      <c r="P23" s="29">
+        <f t="shared" si="1"/>
+        <v>94.896551724137908</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="24" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L24" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="M24" s="30">
+        <f>P2*(R4+R5+R6)/(R1+R3+R4+R5+R6)</f>
+        <v>463.23809523809524</v>
+      </c>
+      <c r="N24" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O24" s="30">
+        <f>(O2/P2)*M24</f>
+        <v>2261.9047619047619</v>
+      </c>
+      <c r="P24" s="30">
+        <f t="shared" si="1"/>
+        <v>48.341543513957333</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>195</v>
+      </c>
+      <c r="M25" s="29">
+        <f>P2*(R4+R5+R6)/(R1+R4+R5+R6)</f>
+        <v>738.83544303797464</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O25" s="33">
+        <f>(O2/P2)*M25</f>
+        <v>3607.5949367088606</v>
+      </c>
+      <c r="P25" s="30">
+        <f t="shared" si="1"/>
+        <v>275.5973477998794</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="26" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>198</v>
+      </c>
+      <c r="M26" s="29">
+        <f>P2*(R5+R6)/(R1+R2+R5+R6)</f>
+        <v>528.87912087912093</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O26" s="33">
+        <f>(O2/P2)*M26</f>
+        <v>2582.4175824175827</v>
+      </c>
+      <c r="P26" s="29">
+        <f t="shared" si="1"/>
+        <v>-209.95632215885371</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="27" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L27" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="M27" s="30">
+        <f>P2*(R4+R5+R6)/(R1+R2+R4+R5+R6)</f>
+        <v>577.90099009900985</v>
+      </c>
+      <c r="N27" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O27" s="30">
+        <f>(O2/P2)*M27</f>
+        <v>2821.7821782178216</v>
+      </c>
+      <c r="P27" s="30">
+        <f t="shared" si="1"/>
+        <v>49.021869219888913</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="28" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="L28" t="s">
+        <v>201</v>
+      </c>
+      <c r="M28" s="29">
+        <f>P2*(R5+R6)/(R1+R5+R6)</f>
+        <v>697.50724637681162</v>
+      </c>
+      <c r="N28" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="O28" s="33">
+        <f>(O2/P2)*M28</f>
+        <v>3405.7971014492755</v>
+      </c>
+      <c r="P28" s="30">
+        <f t="shared" si="1"/>
+        <v>119.60625627780178</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="32" spans="12:17" x14ac:dyDescent="0.25">
+      <c r="P32" s="29"/>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P34" s="29"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>